<commit_message>
Android Studio 查看源代码,提示sources for 'Android xx platform' not found 解决办法
</commit_message>
<xml_diff>
--- a/Document/Android/Android开发.xlsx
+++ b/Document/Android/Android开发.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="3080" windowWidth="25600" windowHeight="16060" tabRatio="822" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="822" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="7" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="1164">
   <si>
     <t>Android Studio</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -20699,6 +20699,205 @@
   </si>
   <si>
     <t xml:space="preserve">  /data/data/&lt;app package&gt;/files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 Android Studio 查看SDK源代码时提示:Sources for 'Android xx Platform' not found</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这些源代码储存在 /Users/&lt;userName&gt;/Library/Android/sdk/sources 下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">如: Android API 19的源代码 储存在  /Users/&lt;userName&gt;/Library/Android/sdk/sources/android-19 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">      Android API 23的源代码 储存在  /Users/&lt;userName&gt;/Library/Android/sdk/sources/android-23 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决办法:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首先要确保已经下载了相关Android API 的源代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如:Android studio 2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    该配置文件包含了JDK的配置,以及不同的Android API Platform 的相关配置,比如关联的源代码,则是在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体 (正文)"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sourcePath 节点</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>设置相应的androi studio软件版本的配置文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体 (正文)"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> jdk.table.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    将源代码的目录所在的路劲拷贝过来,设置sourcePath节点的值,重启Android studio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;/root&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/sourcePath&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>sourcePath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t xml:space="preserve">root </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>type=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>"composite"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t xml:space="preserve">root </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>type=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t xml:space="preserve">"simple" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>url=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>"file://$USER_HOME$/Library/Android/sdk/sources/android-23” /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>其所在的文件的部分代码如下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    该配置文件的路劲为:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体 (正文)"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/Users/&lt;userName&gt;/Library/Preferences/AndroidStudio2.1/options/jdk.table.xml</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20706,7 +20905,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -21031,6 +21230,29 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000080"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF008000"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -21135,7 +21357,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="178">
+  <cellStyleXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -21314,8 +21536,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -21551,8 +21775,24 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="178">
+  <cellStyles count="180">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -21730,6 +21970,8 @@
     <cellStyle name="访问过的超链接" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22818,6 +23060,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="47815500"/>
+          <a:ext cx="10248900" cy="6680200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -35744,7 +36024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -37493,11 +37773,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S235"/>
+  <dimension ref="A1:S260"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A219" sqref="A219"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -38562,6 +38840,165 @@
       </c>
       <c r="E235" s="44"/>
       <c r="F235" s="44"/>
+    </row>
+    <row r="237" spans="3:6">
+      <c r="C237" s="44" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="238" spans="3:6">
+      <c r="C238" s="44"/>
+    </row>
+    <row r="239" spans="3:6">
+      <c r="C239" s="44" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="241" spans="3:16">
+      <c r="C241" s="81">
+        <v>1</v>
+      </c>
+      <c r="D241" s="81" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="242" spans="3:16">
+      <c r="D242" s="81" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="243" spans="3:16">
+      <c r="D243" s="81" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="244" spans="3:16">
+      <c r="D244" s="81" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="246" spans="3:16">
+      <c r="C246" s="81">
+        <v>2</v>
+      </c>
+      <c r="D246" s="81" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="247" spans="3:16">
+      <c r="D247" s="81" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="248" spans="3:16">
+      <c r="D248" s="81" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="250" spans="3:16">
+      <c r="D250" s="81" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="251" spans="3:16">
+      <c r="D251" s="81" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="252" spans="3:16" ht="17">
+      <c r="D252" s="113"/>
+      <c r="E252" s="113"/>
+      <c r="F252" s="113"/>
+    </row>
+    <row r="253" spans="3:16" ht="17">
+      <c r="D253" s="113"/>
+      <c r="E253" s="114" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F253" s="115"/>
+      <c r="G253" s="83"/>
+      <c r="H253" s="83"/>
+      <c r="I253" s="83"/>
+      <c r="J253" s="83"/>
+      <c r="K253" s="83"/>
+      <c r="L253" s="83"/>
+      <c r="M253" s="83"/>
+      <c r="N253" s="83"/>
+      <c r="O253" s="83"/>
+      <c r="P253" s="84"/>
+    </row>
+    <row r="254" spans="3:16" ht="17">
+      <c r="D254" s="113"/>
+      <c r="E254" s="116" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F254" s="117"/>
+      <c r="G254" s="87"/>
+      <c r="H254" s="87"/>
+      <c r="I254" s="87"/>
+      <c r="J254" s="87"/>
+      <c r="K254" s="87"/>
+      <c r="L254" s="87"/>
+      <c r="M254" s="87"/>
+      <c r="N254" s="87"/>
+      <c r="O254" s="87"/>
+      <c r="P254" s="88"/>
+    </row>
+    <row r="255" spans="3:16" ht="17">
+      <c r="D255" s="113"/>
+      <c r="E255" s="116" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F255" s="117"/>
+      <c r="G255" s="87"/>
+      <c r="H255" s="87"/>
+      <c r="I255" s="87"/>
+      <c r="J255" s="87"/>
+      <c r="K255" s="87"/>
+      <c r="L255" s="87"/>
+      <c r="M255" s="87"/>
+      <c r="N255" s="87"/>
+      <c r="O255" s="87"/>
+      <c r="P255" s="88"/>
+    </row>
+    <row r="256" spans="3:16" ht="17">
+      <c r="D256" s="113"/>
+      <c r="E256" s="118" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F256" s="117"/>
+      <c r="G256" s="87"/>
+      <c r="H256" s="87"/>
+      <c r="I256" s="87"/>
+      <c r="J256" s="87"/>
+      <c r="K256" s="87"/>
+      <c r="L256" s="87"/>
+      <c r="M256" s="87"/>
+      <c r="N256" s="87"/>
+      <c r="O256" s="87"/>
+      <c r="P256" s="88"/>
+    </row>
+    <row r="257" spans="4:16" ht="17">
+      <c r="D257" s="113"/>
+      <c r="E257" s="119" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F257" s="120"/>
+      <c r="G257" s="95"/>
+      <c r="H257" s="95"/>
+      <c r="I257" s="95"/>
+      <c r="J257" s="95"/>
+      <c r="K257" s="95"/>
+      <c r="L257" s="95"/>
+      <c r="M257" s="95"/>
+      <c r="N257" s="95"/>
+      <c r="O257" s="95"/>
+      <c r="P257" s="96"/>
+    </row>
+    <row r="260" spans="4:16">
+      <c r="E260" s="81" t="s">
+        <v>1162</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>